<commit_message>
Merging the project for demo
</commit_message>
<xml_diff>
--- a/LMSProject-UIAchievers/src/test/resources/exceldata/UI_lms.xlsx
+++ b/LMSProject-UIAchievers/src/test/resources/exceldata/UI_lms.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>Program Name</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>onedrive/NumpyNinja/SDET150/Videos</t>
+  </si>
+  <si>
+    <t>Selenium Class</t>
   </si>
   <si>
     <t>Jun23-Status200-SDET-API Hackathon-001</t>
@@ -600,38 +603,41 @@
       <c r="M2" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="N2" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="O2" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="W2" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>